<commit_message>
update pdf parser script with tkinter
</commit_message>
<xml_diff>
--- a/parsing_documents/parsePDFs01/output/GSAM_Market_Monitor_081222.xlsx
+++ b/parsing_documents/parsePDFs01/output/GSAM_Market_Monitor_081222.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,1330 +439,1026 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>INDEX RETURNS</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Asset Type</t>
+          <t>Unnamed: 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Index</t>
+          <t>Unnamed: 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1 WEEK</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>MTD</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>QTD</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>YTD</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EQUITIES</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>S&amp;P 500</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3.31%</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>3.71%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>13.27%</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-9.34%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>EQUITIES</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>DJ Industrial Average</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2.99%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2.87%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>9.89%</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-5.98%</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>S&amp;P 500</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>3.31%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Russell 2000</t>
+          <t>3.71%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.97%</t>
+          <t>13.27%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7.03%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>18.21%</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>-9.48%</t>
+          <t>-9.34%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>DJ Industrial Average</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>2.99%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Russell Midcap</t>
+          <t>2.87%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4.19%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.91%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>15.26%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-9.60%</t>
+          <t>-5.98%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Russell 2000</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>4.97%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>STOXX Europe 50 (€)</t>
+          <t>7.03%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.42%</t>
+          <t>18.21%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.92%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>9.53%</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-9.58%</t>
+          <t>-9.48%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Russell Midcap</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>4.19%</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>STOXX Europe 600 (€)†</t>
+          <t>4.91%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.29%</t>
+          <t>15.26%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.74%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>8.54%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-7.71%</t>
+          <t>-9.60%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>STOXX Europe 50 (€)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.42%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MSCI EAFE Small Cap</t>
+          <t>1.92%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.99%</t>
+          <t>9.53%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2.47%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>9.25%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-17.47%</t>
+          <t>-9.58%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>STOXX Europe 600 (€)†</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.29%</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FTSE 100 (£)</t>
+          <t>0.74%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.18%</t>
+          <t>8.54%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.54%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>5.27%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>4.25%</t>
+          <t>-7.71%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI EAFE Small Cap</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>2.99%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DAX (€)</t>
+          <t>2.47%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.63%</t>
+          <t>9.25%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.31%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>7.92%</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>-13.15%</t>
+          <t>-17.47%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>FTSE 100 (£)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.18%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FTSE MIB (€)</t>
+          <t>1.54%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.70%</t>
+          <t>5.27%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.52%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>8.35%</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-12.89%</t>
+          <t>4.25%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>DAX (€)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.63%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CAC 40 (€)†</t>
+          <t>2.31%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.26%</t>
+          <t>7.92%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.63%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>10.76%</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>-6.45%</t>
+          <t>-13.15%</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>FTSE MIB (€)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.70%</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SWISS MKT (CHF)</t>
+          <t>2.52%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>8.35%</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-0.16%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>3.60%</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-11.22%</t>
+          <t>-12.89%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>CAC 40 (€)†</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.26%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TOPIX (¥)</t>
+          <t>1.63%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.34%</t>
+          <t>10.76%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.69%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>5.48%</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0.44%</t>
+          <t>-6.45%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>SWISS MKT (CHF)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>0.05%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Hang Seng (HKD)</t>
+          <t>-0.16%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-0.11%</t>
+          <t>3.60%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.13%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-7.20%</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-11.67%</t>
+          <t>-11.22%</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>TOPIX (¥)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.34%</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MSCI World</t>
+          <t>1.69%</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3.06%</t>
+          <t>5.48%</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3.30%</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>11.54%</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>-11.09%</t>
+          <t>0.44%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Hang Seng (HKD)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>-0.11%</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MSCI China Free†</t>
+          <t>0.13%</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>-0.38%</t>
+          <t>-7.20%</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>-0.01%</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>-8.93%</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-15.12%</t>
+          <t>-11.67%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI World</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>3.06%</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MSCI EAFE</t>
+          <t>3.30%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2.17%</t>
+          <t>11.54%</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.51%</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>6.58%</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>-13.95%</t>
+          <t>-11.09%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI China Free†</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>-0.38%</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MSCI EM</t>
+          <t>-0.01%</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.66%</t>
+          <t>-8.93%</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.65%</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2.49%</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-15.42%</t>
+          <t>-15.12%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI EAFE</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>2.17%</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MSCI Brazil (BRL)</t>
+          <t>1.51%</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6.16%</t>
+          <t>6.58%</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>9.11%</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>14.45%</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>10.53%</t>
+          <t>-13.95%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI EM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.66%</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MSCI India (INR)</t>
+          <t>2.65%</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.69%</t>
+          <t>2.49%</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3.48%</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>13.60%</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2.48%</t>
+          <t>-15.42%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI Brazil (BRL)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>6.16%</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MSCI Russia (RUB)</t>
+          <t>9.11%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>14.45%</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>-100.00%</t>
+          <t>10.53%</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI India (INR)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>1.69%</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bloomberg Aggregate</t>
+          <t>3.48%</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>13.60%</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-0.80%</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>1.63%</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>-8.89%</t>
+          <t>2.48%</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI Russia (RUB)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bloomberg Euro Aggregate</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.32%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-0.51%</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>1.05%</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>-18.37%</t>
+          <t>-100.00%</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
           <t>FIXED INCOME</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Bloomberg US High Yield</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0.94%</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1.60%</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>7.60%</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-7.67%</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Aggregate</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.24%</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bloomberg Euro High Yield (€)</t>
+          <t>-0.80%</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.75%</t>
+          <t>1.63%</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.66%</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>6.83%</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>-8.59%</t>
+          <t>-8.89%</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Euro Aggregate</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.32%</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bloomberg Muni Aggregate</t>
+          <t>-0.51%</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>-0.08%</t>
+          <t>1.05%</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>-0.19%</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2.44%</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-6.76%</t>
+          <t>-18.37%</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg US High Yield</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.94%</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bloomberg TIPS</t>
+          <t>1.60%</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.18%</t>
+          <t>7.60%</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-1.41%</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>3.06%</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-6.90%</t>
+          <t>-7.67%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Euro High Yield (€)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.75%</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JPM EMBI Glbl. Divers.</t>
+          <t>1.66%</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.51%</t>
+          <t>6.83%</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2.43%</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>5.39%</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>-16.01%</t>
+          <t>-8.59%</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Muni Aggregate</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>-0.08%</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JPM GBI-EM Glbl. Divers.</t>
+          <t>-0.19%</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.34%</t>
+          <t>2.44%</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3.09%</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>3.40%</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>-11.63%</t>
+          <t>-6.76%</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg TIPS</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>0.18%</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>DJ US Real Estate</t>
+          <t>-1.41%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4.28%</t>
+          <t>3.06%</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.66%</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>11.77%</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>-10.61%</t>
+          <t>-6.90%</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>JPM EMBI Glbl. Divers.</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>1.51%</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FTSE EPRA/NAREIT Dvlpd. Ex-US</t>
+          <t>2.43%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.89%</t>
+          <t>5.39%</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.83%</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>7.21%</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>-14.36%</t>
+          <t>-16.01%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>JPM GBI-EM Glbl. Divers.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>2.34%</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>S&amp;P GSCI</t>
+          <t>3.09%</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4.45%</t>
+          <t>3.40%</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-1.83%</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>-1.87%</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>33.26%</t>
+          <t>-11.63%</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Alerian MLP *</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>4.95%</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>2.14%</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>14.90%</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>26.43%</t>
-        </is>
-      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>DJ US Real Estate</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>4.28%</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>US Dollar Index</t>
+          <t>2.66%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>-0.91%</t>
+          <t>11.77%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-0.25%</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>0.90%</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>10.59%</t>
+          <t>-10.61%</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>FTSE EPRA/NAREIT Dvlpd. Ex-US</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>2.89%</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>0.83%</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>7.21%</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-14.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>S&amp;P GSCI</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>4.45%</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>-1.83%</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>-1.87%</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>33.26%</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Alerian MLP *</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>4.95%</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2.14%</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>14.90%</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>26.43%</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>US Dollar Index</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>-0.91%</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>-0.25%</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.90%</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>10.59%</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>VIX</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>-7.66%</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>-8.44%</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>-31.97%</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>13.41%</t>
         </is>

</xml_diff>

<commit_message>
Update pdf parser script (#5)
* udpate parssepdf main.py

* update pdf parser script with tkinter
</commit_message>
<xml_diff>
--- a/parsing_documents/parsePDFs01/output/GSAM_Market_Monitor_081222.xlsx
+++ b/parsing_documents/parsePDFs01/output/GSAM_Market_Monitor_081222.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,1330 +439,1026 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>INDEX RETURNS</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Asset Type</t>
+          <t>Unnamed: 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Index</t>
+          <t>Unnamed: 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1 WEEK</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>MTD</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>QTD</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>YTD</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EQUITIES</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>S&amp;P 500</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3.31%</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>3.71%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>13.27%</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-9.34%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>EQUITIES</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>DJ Industrial Average</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2.99%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2.87%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>9.89%</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-5.98%</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>S&amp;P 500</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>3.31%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Russell 2000</t>
+          <t>3.71%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.97%</t>
+          <t>13.27%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7.03%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>18.21%</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>-9.48%</t>
+          <t>-9.34%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>DJ Industrial Average</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>2.99%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Russell Midcap</t>
+          <t>2.87%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4.19%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.91%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>15.26%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-9.60%</t>
+          <t>-5.98%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Russell 2000</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>4.97%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>STOXX Europe 50 (€)</t>
+          <t>7.03%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.42%</t>
+          <t>18.21%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.92%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>9.53%</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-9.58%</t>
+          <t>-9.48%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Russell Midcap</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>4.19%</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>STOXX Europe 600 (€)†</t>
+          <t>4.91%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.29%</t>
+          <t>15.26%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.74%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>8.54%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-7.71%</t>
+          <t>-9.60%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>STOXX Europe 50 (€)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.42%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MSCI EAFE Small Cap</t>
+          <t>1.92%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.99%</t>
+          <t>9.53%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2.47%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>9.25%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-17.47%</t>
+          <t>-9.58%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>STOXX Europe 600 (€)†</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.29%</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FTSE 100 (£)</t>
+          <t>0.74%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.18%</t>
+          <t>8.54%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.54%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>5.27%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>4.25%</t>
+          <t>-7.71%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI EAFE Small Cap</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>2.99%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DAX (€)</t>
+          <t>2.47%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.63%</t>
+          <t>9.25%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.31%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>7.92%</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>-13.15%</t>
+          <t>-17.47%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>FTSE 100 (£)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.18%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FTSE MIB (€)</t>
+          <t>1.54%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.70%</t>
+          <t>5.27%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.52%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>8.35%</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-12.89%</t>
+          <t>4.25%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>DAX (€)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.63%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CAC 40 (€)†</t>
+          <t>2.31%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.26%</t>
+          <t>7.92%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.63%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>10.76%</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>-6.45%</t>
+          <t>-13.15%</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>FTSE MIB (€)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.70%</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SWISS MKT (CHF)</t>
+          <t>2.52%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>8.35%</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-0.16%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>3.60%</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-11.22%</t>
+          <t>-12.89%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>CAC 40 (€)†</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.26%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TOPIX (¥)</t>
+          <t>1.63%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.34%</t>
+          <t>10.76%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.69%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>5.48%</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0.44%</t>
+          <t>-6.45%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>SWISS MKT (CHF)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>0.05%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Hang Seng (HKD)</t>
+          <t>-0.16%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-0.11%</t>
+          <t>3.60%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.13%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-7.20%</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-11.67%</t>
+          <t>-11.22%</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>TOPIX (¥)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.34%</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MSCI World</t>
+          <t>1.69%</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3.06%</t>
+          <t>5.48%</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3.30%</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>11.54%</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>-11.09%</t>
+          <t>0.44%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Hang Seng (HKD)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>-0.11%</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MSCI China Free†</t>
+          <t>0.13%</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>-0.38%</t>
+          <t>-7.20%</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>-0.01%</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>-8.93%</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-15.12%</t>
+          <t>-11.67%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI World</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>3.06%</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MSCI EAFE</t>
+          <t>3.30%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2.17%</t>
+          <t>11.54%</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.51%</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>6.58%</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>-13.95%</t>
+          <t>-11.09%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI China Free†</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>-0.38%</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MSCI EM</t>
+          <t>-0.01%</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.66%</t>
+          <t>-8.93%</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.65%</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2.49%</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-15.42%</t>
+          <t>-15.12%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI EAFE</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>2.17%</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MSCI Brazil (BRL)</t>
+          <t>1.51%</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6.16%</t>
+          <t>6.58%</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>9.11%</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>14.45%</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>10.53%</t>
+          <t>-13.95%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI EM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>1.66%</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MSCI India (INR)</t>
+          <t>2.65%</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.69%</t>
+          <t>2.49%</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3.48%</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>13.60%</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2.48%</t>
+          <t>-15.42%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI Brazil (BRL)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EQUITIES</t>
+          <t>6.16%</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MSCI Russia (RUB)</t>
+          <t>9.11%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>14.45%</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>-100.00%</t>
+          <t>10.53%</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI India (INR)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>1.69%</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bloomberg Aggregate</t>
+          <t>3.48%</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>13.60%</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-0.80%</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>1.63%</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>-8.89%</t>
+          <t>2.48%</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>MSCI Russia (RUB)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bloomberg Euro Aggregate</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.32%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-0.51%</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>1.05%</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>-18.37%</t>
+          <t>-100.00%</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
           <t>FIXED INCOME</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Bloomberg US High Yield</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0.94%</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1.60%</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>7.60%</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-7.67%</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Aggregate</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.24%</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bloomberg Euro High Yield (€)</t>
+          <t>-0.80%</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.75%</t>
+          <t>1.63%</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.66%</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>6.83%</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>-8.59%</t>
+          <t>-8.89%</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Euro Aggregate</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.32%</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bloomberg Muni Aggregate</t>
+          <t>-0.51%</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>-0.08%</t>
+          <t>1.05%</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>-0.19%</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2.44%</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-6.76%</t>
+          <t>-18.37%</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg US High Yield</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.94%</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bloomberg TIPS</t>
+          <t>1.60%</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.18%</t>
+          <t>7.60%</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-1.41%</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>3.06%</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-6.90%</t>
+          <t>-7.67%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Euro High Yield (€)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>0.75%</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JPM EMBI Glbl. Divers.</t>
+          <t>1.66%</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.51%</t>
+          <t>6.83%</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2.43%</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>5.39%</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>-16.01%</t>
+          <t>-8.59%</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg Muni Aggregate</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FIXED INCOME</t>
+          <t>-0.08%</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JPM GBI-EM Glbl. Divers.</t>
+          <t>-0.19%</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.34%</t>
+          <t>2.44%</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3.09%</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>3.40%</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>-11.63%</t>
+          <t>-6.76%</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>Bloomberg TIPS</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>0.18%</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>DJ US Real Estate</t>
+          <t>-1.41%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4.28%</t>
+          <t>3.06%</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.66%</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>11.77%</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>-10.61%</t>
+          <t>-6.90%</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>JPM EMBI Glbl. Divers.</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>1.51%</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FTSE EPRA/NAREIT Dvlpd. Ex-US</t>
+          <t>2.43%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.89%</t>
+          <t>5.39%</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.83%</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>7.21%</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>-14.36%</t>
+          <t>-16.01%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>JPM GBI-EM Glbl. Divers.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>2.34%</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>S&amp;P GSCI</t>
+          <t>3.09%</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4.45%</t>
+          <t>3.40%</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-1.83%</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>-1.87%</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>33.26%</t>
+          <t>-11.63%</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Index Returns</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Alerian MLP *</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>4.95%</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>2.14%</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>14.90%</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>26.43%</t>
-        </is>
-      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>DJ US Real Estate</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>4.28%</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>US Dollar Index</t>
+          <t>2.66%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>-0.91%</t>
+          <t>11.77%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-0.25%</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>0.90%</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>10.59%</t>
+          <t>-10.61%</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Index Returns</t>
+          <t>FTSE EPRA/NAREIT Dvlpd. Ex-US</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>2.89%</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>0.83%</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>7.21%</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-14.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>S&amp;P GSCI</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>4.45%</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>-1.83%</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>-1.87%</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>33.26%</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Alerian MLP *</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>4.95%</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2.14%</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>14.90%</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>26.43%</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>US Dollar Index</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>-0.91%</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>-0.25%</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.90%</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>10.59%</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>VIX</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>-7.66%</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>-8.44%</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>-31.97%</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>13.41%</t>
         </is>

</xml_diff>